<commit_message>
Rectification feuille de route du 07 aout 2023
</commit_message>
<xml_diff>
--- a/Planning/Feuilles de route/Feuilles_de_route_08_07.xlsx
+++ b/Planning/Feuilles de route/Feuilles_de_route_08_07.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fef\Documents\DWWM_22238\ressources\Planning\Feuilles de route\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF883F6A-5345-4DB1-9CD8-2BEA9B032F0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CE7494D-041C-4930-BDBE-12B3F9630335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Lundi</t>
   </si>
@@ -159,6 +159,9 @@
       </rPr>
       <t>Les clauses de sélection</t>
     </r>
+  </si>
+  <si>
+    <t>14h: bilan intermédiaire avec David (Manager de formation)</t>
   </si>
 </sst>
 </file>
@@ -311,7 +314,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -353,6 +356,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -672,7 +678,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -724,14 +730,16 @@
       <c r="F4" s="14"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="9"/>
+      <c r="C5" s="15" t="s">
+        <v>17</v>
+      </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>

</xml_diff>